<commit_message>
Added 2019 Super Rugby Semifinal Forecasts
</commit_message>
<xml_diff>
--- a/2019SuperRugby/Weekly Forecasts/Round_QF_Matrix.xlsx
+++ b/2019SuperRugby/Weekly Forecasts/Round_QF_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RugbyPredictifier\2019SuperRugby\Weekly Forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29CB2C6-F01C-484E-95A5-8779BF1061EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F966B7-217E-4A11-B3DB-45829A4A5CDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="10" r:id="rId1"/>
@@ -612,18 +612,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,6 +700,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1055,16 +1055,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCC1B88-A672-40E8-B2AC-3162D2164F31}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6328125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="3.6328125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="3.6328125" style="26" customWidth="1"/>
     <col min="3" max="3" width="15.6328125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="3.6328125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="3.6328125" style="26" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" style="15" customWidth="1"/>
     <col min="6" max="6" width="3.6328125" style="15" customWidth="1"/>
     <col min="7" max="8" width="15.6328125" style="15" customWidth="1"/>
@@ -1100,10 +1100,10 @@
       <c r="D2" s="14"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="47"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
@@ -1118,10 +1118,10 @@
       <c r="D3" s="14"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="49"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -1137,7 +1137,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="20"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -1146,64 +1146,64 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21">
+      <c r="B5" s="17">
         <v>1</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="37">
         <v>34</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="44" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="24">
+      <c r="K5" s="20">
         <v>2</v>
       </c>
-      <c r="L5" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="45">
+      <c r="L5" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="41">
         <v>31</v>
       </c>
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
-      <c r="B6" s="25">
+      <c r="B6" s="21">
         <v>8</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="38">
         <v>21</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="27">
+      <c r="G6" s="23">
         <v>31</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="24">
         <v>21</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="29">
+      <c r="K6" s="25">
         <v>7</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="46">
+      <c r="M6" s="42">
         <v>27</v>
       </c>
       <c r="N6" s="13"/>
@@ -1212,13 +1212,13 @@
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="13"/>
-      <c r="E7" s="31"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="31"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="32"/>
+      <c r="K7" s="28"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -1227,24 +1227,24 @@
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="21">
+      <c r="D8" s="17">
         <v>1</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="29">
         <v>31</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="24">
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="20">
         <v>2</v>
       </c>
-      <c r="J8" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="33">
+      <c r="J8" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="29">
         <v>26</v>
       </c>
       <c r="L8" s="13"/>
@@ -1255,24 +1255,24 @@
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="25">
+      <c r="D9" s="21">
         <v>4</v>
       </c>
-      <c r="E9" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="28">
+      <c r="E9" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="24">
         <v>20</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="29">
+      <c r="I9" s="25">
         <v>3</v>
       </c>
-      <c r="J9" s="49" t="s">
+      <c r="J9" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="24">
         <v>22</v>
       </c>
       <c r="L9" s="13"/>
@@ -1284,26 +1284,26 @@
       <c r="B10" s="14"/>
       <c r="C10" s="13"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="31"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="32"/>
+      <c r="K10" s="28"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" ht="14" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
-      <c r="B11" s="21">
+      <c r="B11" s="17">
         <v>4</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="43">
+      <c r="C11" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="39">
         <v>26</v>
       </c>
       <c r="E11" s="13"/>
@@ -1312,26 +1312,26 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="24">
+      <c r="K11" s="20">
         <v>3</v>
       </c>
-      <c r="L11" s="49" t="s">
+      <c r="L11" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="45">
+      <c r="M11" s="41">
         <v>22</v>
       </c>
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
-      <c r="B12" s="25">
+      <c r="B12" s="21">
         <v>5</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="40">
         <v>22</v>
       </c>
       <c r="E12" s="13"/>
@@ -1340,13 +1340,13 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="29">
+      <c r="K12" s="25">
         <v>6</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="L12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="46">
+      <c r="M12" s="42">
         <v>20</v>
       </c>
       <c r="N12" s="13"/>
@@ -1381,9 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B46F1B0-2273-49FD-9871-22450F401DFF}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>